<commit_message>
4.5,4.7 Padam templates and Jatai working edits 24/01/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Consolidated Jatai and Ghanam Rules - nmvvvvvv.xlsx
+++ b/TS Jatai Working/Consolidated Jatai and Ghanam Rules - nmvvvvvv.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\texts\TS Jatai Working\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,10 +16,10 @@
     <sheet name="Ghanam" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Ghanam!$C$4:$K$208</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Jatai!$A$1:$R$174</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Ghanam!$B$4:$L$208</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Jatai!$A$3:$K$173</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2961" uniqueCount="1702">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2964" uniqueCount="1704">
   <si>
     <t>Rules Observed from JatA Mani and JatA DarpaNam</t>
   </si>
@@ -5350,18 +5350,30 @@
   <si>
     <t>yad vo# voq yad yad vo# vaqyam ~Mvaqyam voq yad yad vo# vaqyam</t>
   </si>
+  <si>
+    <t>JD-34</t>
+  </si>
+  <si>
+    <t>JD-13</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -5701,319 +5713,319 @@
   </cellStyleXfs>
   <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -6299,13 +6311,13 @@
   <dimension ref="A1:R176"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="G102" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K105" sqref="K105"/>
+      <selection pane="bottomRight" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.140625" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" customWidth="1"/>
@@ -6320,7 +6332,7 @@
     <col min="11" max="11" width="81.140625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="20.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6337,7 +6349,7 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="3" spans="1:18" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="45.75">
       <c r="A3" s="1"/>
       <c r="B3" s="18" t="s">
         <v>1</v>
@@ -6377,7 +6389,7 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" s="14" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" s="14" customFormat="1" ht="30.75">
       <c r="A4" s="1"/>
       <c r="B4" s="9" t="s">
         <v>131</v>
@@ -6413,7 +6425,7 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" s="14" customFormat="1" ht="18">
       <c r="A5" s="1"/>
       <c r="B5" s="9" t="s">
         <v>131</v>
@@ -6449,7 +6461,7 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:18" s="14" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" s="14" customFormat="1" ht="30.75">
       <c r="A6" s="1"/>
       <c r="B6" s="9" t="s">
         <v>131</v>
@@ -6485,7 +6497,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" s="14" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" s="14" customFormat="1" ht="30.75">
       <c r="A7" s="1"/>
       <c r="B7" s="9" t="s">
         <v>148</v>
@@ -6523,7 +6535,7 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" s="14" customFormat="1" ht="18">
       <c r="A8" s="1"/>
       <c r="B8" s="9" t="s">
         <v>148</v>
@@ -6561,7 +6573,7 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" s="14" customFormat="1" ht="18">
       <c r="A9" s="1"/>
       <c r="B9" s="9" t="s">
         <v>148</v>
@@ -6599,7 +6611,7 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" s="14" customFormat="1" ht="18">
       <c r="A10" s="1"/>
       <c r="B10" s="9" t="s">
         <v>148</v>
@@ -6635,7 +6647,7 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" s="14" customFormat="1" ht="18">
       <c r="A11" s="1"/>
       <c r="B11" s="9" t="s">
         <v>148</v>
@@ -6673,7 +6685,7 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" s="14" customFormat="1" ht="18">
       <c r="A12" s="1"/>
       <c r="B12" s="9" t="s">
         <v>148</v>
@@ -6713,7 +6725,7 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" s="14" customFormat="1" ht="18">
       <c r="A13" s="1"/>
       <c r="B13" s="9" t="s">
         <v>148</v>
@@ -6751,7 +6763,7 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" s="14" customFormat="1" ht="18">
       <c r="A14" s="1"/>
       <c r="B14" s="9" t="s">
         <v>148</v>
@@ -6789,7 +6801,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" s="14" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:18" s="14" customFormat="1" ht="28.5">
       <c r="A15" s="1"/>
       <c r="B15" s="9" t="s">
         <v>148</v>
@@ -6815,7 +6827,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" s="14" customFormat="1" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" s="14" customFormat="1" ht="45.75">
       <c r="A16" s="1"/>
       <c r="B16" s="9" t="s">
         <v>148</v>
@@ -6851,7 +6863,7 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="1:18" s="14" customFormat="1" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" s="14" customFormat="1" ht="45.75">
       <c r="A17" s="1"/>
       <c r="B17" s="9" t="s">
         <v>148</v>
@@ -6887,7 +6899,7 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="18" spans="1:18" s="14" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" s="14" customFormat="1" ht="30.75">
       <c r="A18" s="1"/>
       <c r="B18" s="9" t="s">
         <v>148</v>
@@ -6923,7 +6935,7 @@
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
     </row>
-    <row r="19" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" s="14" customFormat="1" ht="18">
       <c r="A19" s="1"/>
       <c r="B19" s="9" t="s">
         <v>148</v>
@@ -6959,7 +6971,7 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
     </row>
-    <row r="20" spans="1:18" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" s="14" customFormat="1" ht="18">
       <c r="A20" s="1"/>
       <c r="B20" s="9" t="s">
         <v>148</v>
@@ -6995,7 +7007,7 @@
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
     </row>
-    <row r="21" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" ht="30.75">
       <c r="A21" s="1"/>
       <c r="B21" s="9" t="s">
         <v>148</v>
@@ -7031,7 +7043,7 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" ht="18">
       <c r="A22" s="1"/>
       <c r="B22" s="9" t="s">
         <v>148</v>
@@ -7067,7 +7079,7 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
     </row>
-    <row r="23" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" ht="30.75">
       <c r="A23" s="1"/>
       <c r="B23" s="9" t="s">
         <v>148</v>
@@ -7103,7 +7115,7 @@
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
     </row>
-    <row r="24" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" ht="30.75">
       <c r="A24" s="1"/>
       <c r="B24" s="9" t="s">
         <v>148</v>
@@ -7139,7 +7151,7 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="1:18" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" ht="60.75">
       <c r="A25" s="1"/>
       <c r="B25" s="9" t="s">
         <v>148</v>
@@ -7177,7 +7189,7 @@
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
     </row>
-    <row r="26" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" ht="30.75">
       <c r="A26" s="1"/>
       <c r="B26" s="9" t="s">
         <v>148</v>
@@ -7215,7 +7227,7 @@
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
     </row>
-    <row r="27" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" ht="30.75">
       <c r="A27" s="1"/>
       <c r="B27" s="9" t="s">
         <v>148</v>
@@ -7253,7 +7265,7 @@
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
     </row>
-    <row r="28" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" ht="30.75">
       <c r="A28" s="1"/>
       <c r="B28" s="9" t="s">
         <v>148</v>
@@ -7291,7 +7303,7 @@
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
     </row>
-    <row r="29" spans="1:18" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" ht="45.75">
       <c r="A29" s="1"/>
       <c r="B29" s="9" t="s">
         <v>148</v>
@@ -7308,9 +7320,11 @@
       <c r="F29" s="61" t="s">
         <v>170</v>
       </c>
-      <c r="G29" s="45"/>
+      <c r="G29" s="61" t="s">
+        <v>1703</v>
+      </c>
       <c r="H29" s="11"/>
-      <c r="I29" s="11" t="s">
+      <c r="I29" s="75" t="s">
         <v>303</v>
       </c>
       <c r="J29" s="25" t="s">
@@ -7327,7 +7341,7 @@
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" ht="18">
       <c r="A30" s="1"/>
       <c r="B30" s="9" t="s">
         <v>148</v>
@@ -7363,7 +7377,7 @@
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" ht="18">
       <c r="A31" s="1"/>
       <c r="B31" s="9" t="s">
         <v>148</v>
@@ -7401,7 +7415,7 @@
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
     </row>
-    <row r="32" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" ht="18">
       <c r="A32" s="1"/>
       <c r="B32" s="9" t="s">
         <v>148</v>
@@ -7439,7 +7453,7 @@
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
     </row>
-    <row r="33" spans="1:18" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" ht="45.75">
       <c r="A33" s="1"/>
       <c r="B33" s="9" t="s">
         <v>148</v>
@@ -7475,7 +7489,7 @@
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
     </row>
-    <row r="34" spans="1:18" ht="75.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" ht="75.75">
       <c r="A34" s="1"/>
       <c r="B34" s="9" t="s">
         <v>148</v>
@@ -7511,7 +7525,7 @@
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
     </row>
-    <row r="35" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" ht="18">
       <c r="A35" s="1"/>
       <c r="B35" s="9" t="s">
         <v>148</v>
@@ -7549,7 +7563,7 @@
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
     </row>
-    <row r="36" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" ht="30.75">
       <c r="A36" s="1"/>
       <c r="B36" s="9" t="s">
         <v>148</v>
@@ -7587,7 +7601,7 @@
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
     </row>
-    <row r="37" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" ht="30.75">
       <c r="A37" s="1"/>
       <c r="B37" s="9" t="s">
         <v>148</v>
@@ -7623,7 +7637,7 @@
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
     </row>
-    <row r="38" spans="1:18" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" ht="45.75">
       <c r="A38" s="1"/>
       <c r="B38" s="9" t="s">
         <v>148</v>
@@ -7659,7 +7673,7 @@
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
     </row>
-    <row r="39" spans="1:18" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" ht="60.75">
       <c r="A39" s="1"/>
       <c r="B39" s="9" t="s">
         <v>148</v>
@@ -7697,7 +7711,7 @@
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
     </row>
-    <row r="40" spans="1:18" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" ht="45.75">
       <c r="A40" s="1"/>
       <c r="B40" s="9" t="s">
         <v>148</v>
@@ -7733,7 +7747,7 @@
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
     </row>
-    <row r="41" spans="1:18" ht="36" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" ht="36">
       <c r="A41" s="1"/>
       <c r="B41" s="9" t="s">
         <v>148</v>
@@ -7750,7 +7764,9 @@
       <c r="F41" s="77" t="s">
         <v>1096</v>
       </c>
-      <c r="G41" s="45"/>
+      <c r="G41" s="61" t="s">
+        <v>1702</v>
+      </c>
       <c r="H41" s="11"/>
       <c r="I41" s="11" t="s">
         <v>299</v>
@@ -7769,7 +7785,7 @@
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
     </row>
-    <row r="42" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" ht="18">
       <c r="A42" s="1"/>
       <c r="B42" s="9" t="s">
         <v>148</v>
@@ -7805,7 +7821,7 @@
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
     </row>
-    <row r="43" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" ht="30.75">
       <c r="A43" s="1"/>
       <c r="B43" s="9" t="s">
         <v>148</v>
@@ -7841,7 +7857,7 @@
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
     </row>
-    <row r="44" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" ht="18">
       <c r="A44" s="1"/>
       <c r="B44" s="9" t="s">
         <v>148</v>
@@ -7877,7 +7893,7 @@
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
     </row>
-    <row r="45" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" ht="18">
       <c r="A45" s="1"/>
       <c r="B45" s="9" t="s">
         <v>148</v>
@@ -7913,7 +7929,7 @@
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
     </row>
-    <row r="46" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" ht="18">
       <c r="A46" s="1"/>
       <c r="B46" s="9" t="s">
         <v>148</v>
@@ -7947,7 +7963,7 @@
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
     </row>
-    <row r="47" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" ht="18">
       <c r="A47" s="1"/>
       <c r="B47" s="9" t="s">
         <v>148</v>
@@ -7985,7 +8001,7 @@
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
     </row>
-    <row r="48" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" ht="30.75">
       <c r="A48" s="1"/>
       <c r="B48" s="9" t="s">
         <v>148</v>
@@ -8021,7 +8037,7 @@
       <c r="Q48" s="1"/>
       <c r="R48" s="1"/>
     </row>
-    <row r="49" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" ht="18">
       <c r="A49" s="1"/>
       <c r="B49" s="9" t="s">
         <v>148</v>
@@ -8057,7 +8073,7 @@
       <c r="Q49" s="1"/>
       <c r="R49" s="1"/>
     </row>
-    <row r="50" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" ht="30.75">
       <c r="A50" s="1"/>
       <c r="B50" s="9" t="s">
         <v>148</v>
@@ -8074,7 +8090,9 @@
       <c r="F50" s="77" t="s">
         <v>1096</v>
       </c>
-      <c r="G50" s="45"/>
+      <c r="G50" s="61" t="s">
+        <v>1702</v>
+      </c>
       <c r="H50" s="11"/>
       <c r="I50" s="11" t="s">
         <v>301</v>
@@ -8093,7 +8111,7 @@
       <c r="Q50" s="1"/>
       <c r="R50" s="1"/>
     </row>
-    <row r="51" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" ht="18">
       <c r="A51" s="1"/>
       <c r="B51" s="9" t="s">
         <v>148</v>
@@ -8131,7 +8149,7 @@
       <c r="Q51" s="1"/>
       <c r="R51" s="1"/>
     </row>
-    <row r="52" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" ht="18">
       <c r="A52" s="1"/>
       <c r="B52" s="9" t="s">
         <v>148</v>
@@ -8169,7 +8187,7 @@
       <c r="Q52" s="1"/>
       <c r="R52" s="1"/>
     </row>
-    <row r="53" spans="1:18" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" ht="60.75">
       <c r="A53" s="1"/>
       <c r="B53" s="9" t="s">
         <v>148</v>
@@ -8207,7 +8225,7 @@
       <c r="Q53" s="1"/>
       <c r="R53" s="1"/>
     </row>
-    <row r="54" spans="1:18" ht="36" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" ht="36">
       <c r="A54" s="1"/>
       <c r="B54" s="9" t="s">
         <v>148</v>
@@ -8245,7 +8263,7 @@
       <c r="Q54" s="1"/>
       <c r="R54" s="1"/>
     </row>
-    <row r="55" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" ht="18">
       <c r="A55" s="1"/>
       <c r="B55" s="9" t="s">
         <v>148</v>
@@ -8283,7 +8301,7 @@
       <c r="Q55" s="1"/>
       <c r="R55" s="1"/>
     </row>
-    <row r="56" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" ht="30.75">
       <c r="A56" s="1"/>
       <c r="B56" s="9" t="s">
         <v>789</v>
@@ -8321,7 +8339,7 @@
       <c r="Q56" s="1"/>
       <c r="R56" s="1"/>
     </row>
-    <row r="57" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" ht="18">
       <c r="A57" s="1"/>
       <c r="B57" s="9" t="s">
         <v>789</v>
@@ -8355,7 +8373,7 @@
       <c r="Q57" s="1"/>
       <c r="R57" s="1"/>
     </row>
-    <row r="58" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" ht="30.75">
       <c r="A58" s="1"/>
       <c r="B58" s="9" t="s">
         <v>789</v>
@@ -8393,7 +8411,7 @@
       <c r="Q58" s="1"/>
       <c r="R58" s="1"/>
     </row>
-    <row r="59" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" ht="18">
       <c r="A59" s="1"/>
       <c r="B59" s="9" t="s">
         <v>789</v>
@@ -8431,7 +8449,7 @@
       <c r="Q59" s="1"/>
       <c r="R59" s="1"/>
     </row>
-    <row r="60" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" ht="18">
       <c r="A60" s="1"/>
       <c r="B60" s="9" t="s">
         <v>789</v>
@@ -8469,7 +8487,7 @@
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
     </row>
-    <row r="61" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" ht="18">
       <c r="A61" s="1"/>
       <c r="B61" s="9" t="s">
         <v>789</v>
@@ -8507,7 +8525,7 @@
       <c r="Q61" s="1"/>
       <c r="R61" s="1"/>
     </row>
-    <row r="62" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" ht="18">
       <c r="A62" s="1"/>
       <c r="B62" s="8" t="s">
         <v>789</v>
@@ -8541,7 +8559,7 @@
       <c r="Q62" s="1"/>
       <c r="R62" s="1"/>
     </row>
-    <row r="63" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" ht="18">
       <c r="A63" s="1"/>
       <c r="B63" s="137" t="s">
         <v>15</v>
@@ -8577,7 +8595,7 @@
       <c r="Q63" s="1"/>
       <c r="R63" s="1"/>
     </row>
-    <row r="64" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" ht="18">
       <c r="A64" s="1"/>
       <c r="B64" s="137" t="s">
         <v>15</v>
@@ -8613,7 +8631,7 @@
       <c r="Q64" s="1"/>
       <c r="R64" s="1"/>
     </row>
-    <row r="65" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" ht="18">
       <c r="A65" s="1"/>
       <c r="B65" s="137" t="s">
         <v>15</v>
@@ -8649,7 +8667,7 @@
       <c r="Q65" s="1"/>
       <c r="R65" s="1"/>
     </row>
-    <row r="66" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" ht="18">
       <c r="A66" s="1"/>
       <c r="B66" s="137" t="s">
         <v>15</v>
@@ -8683,7 +8701,7 @@
       <c r="Q66" s="1"/>
       <c r="R66" s="1"/>
     </row>
-    <row r="67" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" ht="30.75">
       <c r="A67" s="1"/>
       <c r="B67" s="9" t="s">
         <v>98</v>
@@ -8719,7 +8737,7 @@
       <c r="Q67" s="1"/>
       <c r="R67" s="1"/>
     </row>
-    <row r="68" spans="1:18" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" ht="60.75">
       <c r="A68" s="1"/>
       <c r="B68" s="9" t="s">
         <v>98</v>
@@ -8757,7 +8775,7 @@
       <c r="Q68" s="1"/>
       <c r="R68" s="1"/>
     </row>
-    <row r="69" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" ht="30.75">
       <c r="A69" s="1"/>
       <c r="B69" s="9" t="s">
         <v>98</v>
@@ -8795,7 +8813,7 @@
       <c r="Q69" s="1"/>
       <c r="R69" s="1"/>
     </row>
-    <row r="70" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" ht="30.75">
       <c r="A70" s="1"/>
       <c r="B70" s="9" t="s">
         <v>98</v>
@@ -8831,7 +8849,7 @@
       <c r="Q70" s="1"/>
       <c r="R70" s="1"/>
     </row>
-    <row r="71" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" ht="18">
       <c r="A71" s="1"/>
       <c r="B71" s="9" t="s">
         <v>98</v>
@@ -8871,7 +8889,7 @@
       <c r="Q71" s="1"/>
       <c r="R71" s="1"/>
     </row>
-    <row r="72" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" ht="18">
       <c r="A72" s="1"/>
       <c r="B72" s="9" t="s">
         <v>98</v>
@@ -8909,7 +8927,7 @@
       <c r="Q72" s="1"/>
       <c r="R72" s="1"/>
     </row>
-    <row r="73" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" ht="30.75">
       <c r="A73" s="1"/>
       <c r="B73" s="9" t="s">
         <v>98</v>
@@ -8947,7 +8965,7 @@
       <c r="Q73" s="1"/>
       <c r="R73" s="1"/>
     </row>
-    <row r="74" spans="1:18" ht="35.25" x14ac:dyDescent="0.7">
+    <row r="74" spans="1:18" ht="27">
       <c r="A74" s="1"/>
       <c r="B74" s="9" t="s">
         <v>1331</v>
@@ -8985,7 +9003,7 @@
       <c r="Q74" s="1"/>
       <c r="R74" s="1"/>
     </row>
-    <row r="75" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" ht="30.75">
       <c r="A75" s="1"/>
       <c r="B75" s="9" t="s">
         <v>1331</v>
@@ -9023,7 +9041,7 @@
       <c r="Q75" s="1"/>
       <c r="R75" s="1"/>
     </row>
-    <row r="76" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" ht="18">
       <c r="A76" s="1"/>
       <c r="B76" s="9" t="s">
         <v>1331</v>
@@ -9059,7 +9077,7 @@
       <c r="Q76" s="1"/>
       <c r="R76" s="1"/>
     </row>
-    <row r="77" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" ht="30.75">
       <c r="A77" s="1"/>
       <c r="B77" s="9" t="s">
         <v>1331</v>
@@ -9097,7 +9115,7 @@
       <c r="Q77" s="1"/>
       <c r="R77" s="1"/>
     </row>
-    <row r="78" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" ht="30.75">
       <c r="A78" s="1"/>
       <c r="B78" s="9" t="s">
         <v>1331</v>
@@ -9135,7 +9153,7 @@
       <c r="Q78" s="1"/>
       <c r="R78" s="1"/>
     </row>
-    <row r="79" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" ht="30.75">
       <c r="A79" s="1"/>
       <c r="B79" s="9" t="s">
         <v>139</v>
@@ -9173,7 +9191,7 @@
       <c r="Q79" s="1"/>
       <c r="R79" s="1"/>
     </row>
-    <row r="80" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" ht="18">
       <c r="A80" s="1"/>
       <c r="B80" s="9" t="s">
         <v>139</v>
@@ -9211,7 +9229,7 @@
       <c r="Q80" s="1"/>
       <c r="R80" s="1"/>
     </row>
-    <row r="81" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" ht="18">
       <c r="A81" s="1"/>
       <c r="B81" s="9" t="s">
         <v>139</v>
@@ -9249,7 +9267,7 @@
       <c r="Q81" s="1"/>
       <c r="R81" s="1"/>
     </row>
-    <row r="82" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" ht="30.75">
       <c r="A82" s="1"/>
       <c r="B82" s="9" t="s">
         <v>139</v>
@@ -9287,7 +9305,7 @@
       <c r="Q82" s="1"/>
       <c r="R82" s="1"/>
     </row>
-    <row r="83" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" ht="18">
       <c r="A83" s="1"/>
       <c r="B83" s="9" t="s">
         <v>1310</v>
@@ -9325,7 +9343,7 @@
       <c r="Q83" s="1"/>
       <c r="R83" s="1"/>
     </row>
-    <row r="84" spans="1:18" ht="36" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" ht="36">
       <c r="A84" s="1"/>
       <c r="B84" s="9" t="s">
         <v>1310</v>
@@ -9363,7 +9381,7 @@
       <c r="Q84" s="1"/>
       <c r="R84" s="1"/>
     </row>
-    <row r="85" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" ht="18">
       <c r="A85" s="1"/>
       <c r="B85" s="9" t="s">
         <v>1310</v>
@@ -9403,7 +9421,7 @@
       <c r="Q85" s="1"/>
       <c r="R85" s="1"/>
     </row>
-    <row r="86" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" ht="30.75">
       <c r="A86" s="1"/>
       <c r="B86" s="9" t="s">
         <v>1310</v>
@@ -9424,7 +9442,7 @@
       <c r="H86" s="11" t="s">
         <v>1681</v>
       </c>
-      <c r="I86" s="21" t="s">
+      <c r="I86" s="76" t="s">
         <v>329</v>
       </c>
       <c r="J86" s="25" t="s">
@@ -9441,7 +9459,7 @@
       <c r="Q86" s="1"/>
       <c r="R86" s="1"/>
     </row>
-    <row r="87" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" ht="30.75">
       <c r="A87" s="1"/>
       <c r="B87" s="9" t="s">
         <v>1310</v>
@@ -9477,7 +9495,7 @@
       <c r="Q87" s="1"/>
       <c r="R87" s="1"/>
     </row>
-    <row r="88" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:18" ht="18">
       <c r="A88" s="1"/>
       <c r="B88" s="9" t="s">
         <v>1310</v>
@@ -9513,7 +9531,7 @@
       <c r="Q88" s="1"/>
       <c r="R88" s="1"/>
     </row>
-    <row r="89" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" ht="30.75">
       <c r="A89" s="1"/>
       <c r="B89" s="9" t="s">
         <v>7</v>
@@ -9549,7 +9567,7 @@
       <c r="Q89" s="1"/>
       <c r="R89" s="1"/>
     </row>
-    <row r="90" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" ht="30.75">
       <c r="A90" s="1"/>
       <c r="B90" s="9" t="s">
         <v>7</v>
@@ -9585,7 +9603,7 @@
       <c r="Q90" s="1"/>
       <c r="R90" s="1"/>
     </row>
-    <row r="91" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:18" ht="30.75">
       <c r="A91" s="1"/>
       <c r="B91" s="9" t="s">
         <v>7</v>
@@ -9621,7 +9639,7 @@
       <c r="Q91" s="1"/>
       <c r="R91" s="1"/>
     </row>
-    <row r="92" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:18" ht="30.75">
       <c r="A92" s="1"/>
       <c r="B92" s="9" t="s">
         <v>7</v>
@@ -9657,7 +9675,7 @@
       <c r="Q92" s="1"/>
       <c r="R92" s="1"/>
     </row>
-    <row r="93" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:18" ht="18">
       <c r="A93" s="1"/>
       <c r="B93" s="8" t="s">
         <v>7</v>
@@ -9693,7 +9711,7 @@
       <c r="Q93" s="1"/>
       <c r="R93" s="1"/>
     </row>
-    <row r="94" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:18" ht="18">
       <c r="A94" s="1"/>
       <c r="B94" s="8" t="s">
         <v>7</v>
@@ -9731,7 +9749,7 @@
       <c r="Q94" s="1"/>
       <c r="R94" s="1"/>
     </row>
-    <row r="95" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:18" ht="18">
       <c r="A95" s="1"/>
       <c r="B95" s="8" t="s">
         <v>7</v>
@@ -9767,7 +9785,7 @@
       <c r="Q95" s="1"/>
       <c r="R95" s="1"/>
     </row>
-    <row r="96" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:18" ht="30.75">
       <c r="A96" s="1"/>
       <c r="B96" s="9" t="s">
         <v>7</v>
@@ -9805,7 +9823,7 @@
       <c r="Q96" s="1"/>
       <c r="R96" s="1"/>
     </row>
-    <row r="97" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:18" ht="18">
       <c r="A97" s="1"/>
       <c r="B97" s="9" t="s">
         <v>7</v>
@@ -9841,7 +9859,7 @@
       <c r="Q97" s="1"/>
       <c r="R97" s="1"/>
     </row>
-    <row r="98" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:18" ht="18">
       <c r="A98" s="1"/>
       <c r="B98" s="9" t="s">
         <v>7</v>
@@ -9879,7 +9897,7 @@
       <c r="Q98" s="1"/>
       <c r="R98" s="1"/>
     </row>
-    <row r="99" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:18" ht="18">
       <c r="A99" s="1"/>
       <c r="B99" s="9" t="s">
         <v>7</v>
@@ -9917,7 +9935,7 @@
       <c r="Q99" s="1"/>
       <c r="R99" s="1"/>
     </row>
-    <row r="100" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:18" ht="30.75">
       <c r="A100" s="1"/>
       <c r="B100" s="8" t="s">
         <v>7</v>
@@ -9953,7 +9971,7 @@
       <c r="Q100" s="1"/>
       <c r="R100" s="1"/>
     </row>
-    <row r="101" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:18" ht="30.75">
       <c r="A101" s="1"/>
       <c r="B101" s="9" t="s">
         <v>7</v>
@@ -9993,7 +10011,7 @@
       <c r="Q101" s="1"/>
       <c r="R101" s="1"/>
     </row>
-    <row r="102" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:18" ht="18">
       <c r="A102" s="1"/>
       <c r="B102" s="9" t="s">
         <v>7</v>
@@ -10031,7 +10049,7 @@
       <c r="Q102" s="1"/>
       <c r="R102" s="1"/>
     </row>
-    <row r="103" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:18" ht="30.75">
       <c r="A103" s="1"/>
       <c r="B103" s="9" t="s">
         <v>7</v>
@@ -10069,7 +10087,7 @@
       <c r="Q103" s="1"/>
       <c r="R103" s="1"/>
     </row>
-    <row r="104" spans="1:18" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:18" ht="45.75">
       <c r="A104" s="1"/>
       <c r="B104" s="9" t="s">
         <v>7</v>
@@ -10107,7 +10125,7 @@
       <c r="Q104" s="1"/>
       <c r="R104" s="1"/>
     </row>
-    <row r="105" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:18" ht="30.75">
       <c r="A105" s="1"/>
       <c r="B105" s="9" t="s">
         <v>7</v>
@@ -10145,7 +10163,7 @@
       <c r="Q105" s="1"/>
       <c r="R105" s="1"/>
     </row>
-    <row r="106" spans="1:18" ht="36" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:18" ht="36">
       <c r="A106" s="1"/>
       <c r="B106" s="9" t="s">
         <v>7</v>
@@ -10183,7 +10201,7 @@
       <c r="Q106" s="1"/>
       <c r="R106" s="1"/>
     </row>
-    <row r="107" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:18" ht="18">
       <c r="A107" s="1"/>
       <c r="B107" s="9" t="s">
         <v>7</v>
@@ -10221,7 +10239,7 @@
       <c r="Q107" s="1"/>
       <c r="R107" s="1"/>
     </row>
-    <row r="108" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:18" ht="18">
       <c r="A108" s="1" t="s">
         <v>1161</v>
       </c>
@@ -10259,7 +10277,7 @@
       <c r="Q108" s="1"/>
       <c r="R108" s="1"/>
     </row>
-    <row r="109" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:18" ht="18.75" thickBot="1">
       <c r="A109" s="1"/>
       <c r="B109" s="9" t="s">
         <v>7</v>
@@ -10295,7 +10313,7 @@
       <c r="Q109" s="1"/>
       <c r="R109" s="1"/>
     </row>
-    <row r="110" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:18" ht="31.5" thickBot="1">
       <c r="A110" s="1"/>
       <c r="B110" s="9" t="s">
         <v>7</v>
@@ -10333,7 +10351,7 @@
       <c r="Q110" s="1"/>
       <c r="R110" s="1"/>
     </row>
-    <row r="111" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:18" ht="31.5" thickBot="1">
       <c r="A111" s="1"/>
       <c r="B111" s="9" t="s">
         <v>7</v>
@@ -10369,7 +10387,7 @@
       <c r="Q111" s="1"/>
       <c r="R111" s="1"/>
     </row>
-    <row r="112" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:18" ht="18.75" thickBot="1">
       <c r="A112" s="1"/>
       <c r="B112" s="9" t="s">
         <v>7</v>
@@ -10407,7 +10425,7 @@
       <c r="Q112" s="1"/>
       <c r="R112" s="1"/>
     </row>
-    <row r="113" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:18" ht="18.75" thickBot="1">
       <c r="A113" s="1"/>
       <c r="B113" s="9" t="s">
         <v>7</v>
@@ -10447,7 +10465,7 @@
       <c r="Q113" s="1"/>
       <c r="R113" s="1"/>
     </row>
-    <row r="114" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:18" ht="30.75">
       <c r="A114" s="1"/>
       <c r="B114" s="9" t="s">
         <v>7</v>
@@ -10487,7 +10505,7 @@
       <c r="Q114" s="1"/>
       <c r="R114" s="1"/>
     </row>
-    <row r="115" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:18" ht="18">
       <c r="A115" s="1"/>
       <c r="B115" s="9" t="s">
         <v>7</v>
@@ -10525,7 +10543,7 @@
       <c r="Q115" s="1"/>
       <c r="R115" s="1"/>
     </row>
-    <row r="116" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:18" ht="18">
       <c r="A116" s="1"/>
       <c r="B116" s="9" t="s">
         <v>7</v>
@@ -10561,7 +10579,7 @@
       <c r="Q116" s="1"/>
       <c r="R116" s="1"/>
     </row>
-    <row r="117" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:18" ht="18">
       <c r="A117" s="1"/>
       <c r="B117" s="9" t="s">
         <v>7</v>
@@ -10597,7 +10615,7 @@
       <c r="Q117" s="1"/>
       <c r="R117" s="1"/>
     </row>
-    <row r="118" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:18" ht="18">
       <c r="A118" s="1"/>
       <c r="B118" s="9" t="s">
         <v>19</v>
@@ -10637,7 +10655,7 @@
       <c r="Q118" s="1"/>
       <c r="R118" s="1"/>
     </row>
-    <row r="119" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:18" ht="18">
       <c r="A119" s="1"/>
       <c r="B119" s="63" t="s">
         <v>19</v>
@@ -10675,7 +10693,7 @@
       <c r="Q119" s="1"/>
       <c r="R119" s="1"/>
     </row>
-    <row r="120" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:18" ht="18">
       <c r="A120" s="1"/>
       <c r="B120" s="63" t="s">
         <v>19</v>
@@ -10709,7 +10727,7 @@
       <c r="Q120" s="1"/>
       <c r="R120" s="1"/>
     </row>
-    <row r="121" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:18" ht="18">
       <c r="A121" s="1"/>
       <c r="B121" s="63" t="s">
         <v>19</v>
@@ -10743,7 +10761,7 @@
       <c r="Q121" s="1"/>
       <c r="R121" s="1"/>
     </row>
-    <row r="122" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:18" ht="18.75" thickBot="1">
       <c r="A122" s="1"/>
       <c r="B122" s="63" t="s">
         <v>19</v>
@@ -10777,7 +10795,7 @@
       <c r="Q122" s="1"/>
       <c r="R122" s="1"/>
     </row>
-    <row r="123" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:18" ht="18.75" thickBot="1">
       <c r="A123" s="1"/>
       <c r="B123" s="63" t="s">
         <v>19</v>
@@ -10811,7 +10829,7 @@
       <c r="Q123" s="1"/>
       <c r="R123" s="1"/>
     </row>
-    <row r="124" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:18" ht="18.75" thickBot="1">
       <c r="A124" s="1"/>
       <c r="B124" s="63" t="s">
         <v>19</v>
@@ -10845,7 +10863,7 @@
       <c r="Q124" s="1"/>
       <c r="R124" s="1"/>
     </row>
-    <row r="125" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:18" ht="31.5" thickBot="1">
       <c r="A125" s="1"/>
       <c r="B125" s="63" t="s">
         <v>19</v>
@@ -10879,7 +10897,7 @@
       <c r="Q125" s="1"/>
       <c r="R125" s="1"/>
     </row>
-    <row r="126" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:18" ht="31.5" thickBot="1">
       <c r="A126" s="1"/>
       <c r="B126" s="63" t="s">
         <v>19</v>
@@ -10913,7 +10931,7 @@
       <c r="Q126" s="1"/>
       <c r="R126" s="1"/>
     </row>
-    <row r="127" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:18" ht="18.75" thickBot="1">
       <c r="A127" s="1"/>
       <c r="B127" s="63" t="s">
         <v>19</v>
@@ -10947,7 +10965,7 @@
       <c r="Q127" s="1"/>
       <c r="R127" s="1"/>
     </row>
-    <row r="128" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:18" ht="18.75" thickBot="1">
       <c r="A128" s="1"/>
       <c r="B128" s="63" t="s">
         <v>19</v>
@@ -10981,7 +10999,7 @@
       <c r="Q128" s="1"/>
       <c r="R128" s="1"/>
     </row>
-    <row r="129" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:18" ht="31.5" thickBot="1">
       <c r="A129" s="1"/>
       <c r="B129" s="63" t="s">
         <v>19</v>
@@ -11015,7 +11033,7 @@
       <c r="Q129" s="1"/>
       <c r="R129" s="1"/>
     </row>
-    <row r="130" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:18" ht="30.75">
       <c r="A130" s="1"/>
       <c r="B130" s="9" t="s">
         <v>19</v>
@@ -11051,7 +11069,7 @@
       <c r="Q130" s="1"/>
       <c r="R130" s="1"/>
     </row>
-    <row r="131" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:18" ht="18">
       <c r="A131" s="1"/>
       <c r="B131" s="9" t="s">
         <v>19</v>
@@ -11087,7 +11105,7 @@
       <c r="Q131" s="1"/>
       <c r="R131" s="1"/>
     </row>
-    <row r="132" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:18" ht="18">
       <c r="A132" s="1"/>
       <c r="B132" s="9" t="s">
         <v>19</v>
@@ -11121,7 +11139,7 @@
       <c r="Q132" s="1"/>
       <c r="R132" s="1"/>
     </row>
-    <row r="133" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:18" ht="18">
       <c r="A133" s="1"/>
       <c r="B133" s="9" t="s">
         <v>19</v>
@@ -11155,7 +11173,7 @@
       <c r="Q133" s="1"/>
       <c r="R133" s="1"/>
     </row>
-    <row r="134" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:18" ht="30.75">
       <c r="A134" s="1"/>
       <c r="B134" s="9" t="s">
         <v>19</v>
@@ -11189,7 +11207,7 @@
       <c r="Q134" s="1"/>
       <c r="R134" s="1"/>
     </row>
-    <row r="135" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:18" ht="18">
       <c r="A135" s="1"/>
       <c r="B135" s="9" t="s">
         <v>19</v>
@@ -11223,7 +11241,7 @@
       <c r="Q135" s="1"/>
       <c r="R135" s="1"/>
     </row>
-    <row r="136" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:18" ht="18">
       <c r="A136" s="1"/>
       <c r="B136" s="9" t="s">
         <v>19</v>
@@ -11257,7 +11275,7 @@
       <c r="Q136" s="1"/>
       <c r="R136" s="1"/>
     </row>
-    <row r="137" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:18" ht="18">
       <c r="A137" s="1"/>
       <c r="B137" s="9" t="s">
         <v>19</v>
@@ -11291,7 +11309,7 @@
       <c r="Q137" s="1"/>
       <c r="R137" s="1"/>
     </row>
-    <row r="138" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:18" ht="18">
       <c r="A138" s="1"/>
       <c r="B138" s="9" t="s">
         <v>19</v>
@@ -11325,7 +11343,7 @@
       <c r="Q138" s="1"/>
       <c r="R138" s="1"/>
     </row>
-    <row r="139" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:18" ht="18.75" thickBot="1">
       <c r="A139" s="1"/>
       <c r="B139" s="9" t="s">
         <v>19</v>
@@ -11359,7 +11377,7 @@
       <c r="Q139" s="1"/>
       <c r="R139" s="1"/>
     </row>
-    <row r="140" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:18" ht="18.75" thickBot="1">
       <c r="A140" s="1"/>
       <c r="B140" s="9" t="s">
         <v>19</v>
@@ -11395,7 +11413,7 @@
       <c r="Q140" s="1"/>
       <c r="R140" s="1"/>
     </row>
-    <row r="141" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:18" ht="18">
       <c r="A141" s="1"/>
       <c r="B141" s="9" t="s">
         <v>19</v>
@@ -11431,7 +11449,7 @@
       <c r="Q141" s="1"/>
       <c r="R141" s="1"/>
     </row>
-    <row r="142" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:18" ht="18">
       <c r="A142" s="1"/>
       <c r="B142" s="9" t="s">
         <v>19</v>
@@ -11467,7 +11485,7 @@
       <c r="Q142" s="1"/>
       <c r="R142" s="1"/>
     </row>
-    <row r="143" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:18" ht="18">
       <c r="A143" s="1"/>
       <c r="B143" s="9" t="s">
         <v>19</v>
@@ -11503,7 +11521,7 @@
       <c r="Q143" s="1"/>
       <c r="R143" s="1"/>
     </row>
-    <row r="144" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:18" ht="18">
       <c r="A144" s="1"/>
       <c r="B144" s="9" t="s">
         <v>19</v>
@@ -11537,7 +11555,7 @@
       <c r="Q144" s="1"/>
       <c r="R144" s="1"/>
     </row>
-    <row r="145" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:18" ht="18">
       <c r="A145" s="1"/>
       <c r="B145" s="8" t="s">
         <v>60</v>
@@ -11575,7 +11593,7 @@
       <c r="Q145" s="1"/>
       <c r="R145" s="1"/>
     </row>
-    <row r="146" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:18" ht="30.75">
       <c r="A146" s="1"/>
       <c r="B146" s="8" t="s">
         <v>60</v>
@@ -11613,7 +11631,7 @@
       <c r="Q146" s="1"/>
       <c r="R146" s="1"/>
     </row>
-    <row r="147" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:18" ht="30.75">
       <c r="A147" s="1"/>
       <c r="B147" s="8" t="s">
         <v>60</v>
@@ -11651,7 +11669,7 @@
       <c r="Q147" s="1"/>
       <c r="R147" s="1"/>
     </row>
-    <row r="148" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:18" ht="18.75" thickBot="1">
       <c r="A148" s="1"/>
       <c r="B148" s="9" t="s">
         <v>60</v>
@@ -11689,7 +11707,7 @@
       <c r="Q148" s="1"/>
       <c r="R148" s="1"/>
     </row>
-    <row r="149" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:18" ht="31.5" thickBot="1">
       <c r="A149" s="1"/>
       <c r="B149" s="9" t="s">
         <v>60</v>
@@ -11726,7 +11744,7 @@
       <c r="Q149" s="1"/>
       <c r="R149" s="1"/>
     </row>
-    <row r="150" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:18" ht="18.75" thickBot="1">
       <c r="A150" s="1"/>
       <c r="B150" s="9" t="s">
         <v>60</v>
@@ -11763,7 +11781,7 @@
       <c r="Q150" s="1"/>
       <c r="R150" s="1"/>
     </row>
-    <row r="151" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:18" ht="30.75">
       <c r="A151" s="1"/>
       <c r="B151" s="9" t="s">
         <v>60</v>
@@ -11798,7 +11816,7 @@
       <c r="Q151" s="1"/>
       <c r="R151" s="1"/>
     </row>
-    <row r="152" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:18" ht="30.75">
       <c r="A152" s="1"/>
       <c r="B152" s="8" t="s">
         <v>60</v>
@@ -11829,7 +11847,7 @@
       <c r="Q152" s="1"/>
       <c r="R152" s="1"/>
     </row>
-    <row r="153" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:18" ht="18">
       <c r="A153" s="1"/>
       <c r="B153" s="8" t="s">
         <v>60</v>
@@ -11864,7 +11882,7 @@
       <c r="Q153" s="1"/>
       <c r="R153" s="1"/>
     </row>
-    <row r="154" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:18" ht="18">
       <c r="A154" s="1"/>
       <c r="B154" s="8" t="s">
         <v>60</v>
@@ -11899,7 +11917,7 @@
       <c r="Q154" s="1"/>
       <c r="R154" s="1"/>
     </row>
-    <row r="155" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:18" ht="30.75">
       <c r="A155" s="1"/>
       <c r="B155" s="9" t="s">
         <v>60</v>
@@ -11936,7 +11954,7 @@
       <c r="Q155" s="1"/>
       <c r="R155" s="1"/>
     </row>
-    <row r="156" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:18" ht="18">
       <c r="A156" s="1"/>
       <c r="B156" s="9" t="s">
         <v>60</v>
@@ -11973,7 +11991,7 @@
       <c r="Q156" s="1"/>
       <c r="R156" s="1"/>
     </row>
-    <row r="157" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:18" ht="30.75">
       <c r="A157" s="1"/>
       <c r="B157" s="9" t="s">
         <v>717</v>
@@ -12008,7 +12026,7 @@
       <c r="Q157" s="1"/>
       <c r="R157" s="1"/>
     </row>
-    <row r="158" spans="1:18" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:18" ht="30.6" customHeight="1">
       <c r="A158" s="1"/>
       <c r="B158" s="9" t="s">
         <v>717</v>
@@ -12043,7 +12061,7 @@
       <c r="Q158" s="1"/>
       <c r="R158" s="1"/>
     </row>
-    <row r="159" spans="1:18" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:18" ht="30.75">
       <c r="A159" s="1"/>
       <c r="B159" s="9" t="s">
         <v>717</v>
@@ -12078,7 +12096,7 @@
       <c r="Q159" s="1"/>
       <c r="R159" s="1"/>
     </row>
-    <row r="160" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:18" ht="18.75" thickBot="1">
       <c r="A160" s="1"/>
       <c r="B160" s="9" t="s">
         <v>717</v>
@@ -12115,7 +12133,7 @@
       <c r="Q160" s="1"/>
       <c r="R160" s="1"/>
     </row>
-    <row r="161" spans="1:18" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:18" ht="36.75" thickBot="1">
       <c r="A161" s="1"/>
       <c r="B161" s="9" t="s">
         <v>717</v>
@@ -12152,7 +12170,7 @@
       <c r="Q161" s="1"/>
       <c r="R161" s="1"/>
     </row>
-    <row r="162" spans="1:18" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:18" ht="46.5" thickBot="1">
       <c r="A162" s="1"/>
       <c r="B162" s="9" t="s">
         <v>717</v>
@@ -12187,7 +12205,7 @@
       <c r="Q162" s="1"/>
       <c r="R162" s="1"/>
     </row>
-    <row r="163" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:18" ht="18.75" thickBot="1">
       <c r="A163" s="1"/>
       <c r="B163" s="8" t="s">
         <v>717</v>
@@ -12220,7 +12238,7 @@
       <c r="Q163" s="1"/>
       <c r="R163" s="1"/>
     </row>
-    <row r="164" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:18" ht="18.75" thickBot="1">
       <c r="A164" s="1"/>
       <c r="B164" s="8" t="s">
         <v>717</v>
@@ -12253,7 +12271,7 @@
       <c r="Q164" s="1"/>
       <c r="R164" s="1"/>
     </row>
-    <row r="165" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:18" ht="18.75" thickBot="1">
       <c r="A165" s="1"/>
       <c r="B165" s="9" t="s">
         <v>717</v>
@@ -12286,7 +12304,7 @@
       <c r="Q165" s="1"/>
       <c r="R165" s="1"/>
     </row>
-    <row r="166" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:18" ht="31.5" thickBot="1">
       <c r="A166" s="1"/>
       <c r="B166" s="9" t="s">
         <v>717</v>
@@ -12321,7 +12339,7 @@
       <c r="Q166" s="1"/>
       <c r="R166" s="1"/>
     </row>
-    <row r="167" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:18" ht="31.5" thickBot="1">
       <c r="A167" s="1"/>
       <c r="B167" s="9" t="s">
         <v>717</v>
@@ -12350,7 +12368,7 @@
       <c r="Q167" s="1"/>
       <c r="R167" s="1"/>
     </row>
-    <row r="168" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:18" ht="18.75" thickBot="1">
       <c r="A168" s="1"/>
       <c r="B168" s="9" t="s">
         <v>717</v>
@@ -12385,7 +12403,7 @@
       <c r="Q168" s="1"/>
       <c r="R168" s="1"/>
     </row>
-    <row r="169" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:18" ht="31.5" thickBot="1">
       <c r="A169" s="1"/>
       <c r="B169" s="9" t="s">
         <v>717</v>
@@ -12420,7 +12438,7 @@
       <c r="Q169" s="1"/>
       <c r="R169" s="1"/>
     </row>
-    <row r="170" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:18" ht="18.75" thickBot="1">
       <c r="A170" s="1"/>
       <c r="B170" s="9" t="s">
         <v>717</v>
@@ -12456,7 +12474,7 @@
       <c r="Q170" s="1"/>
       <c r="R170" s="1"/>
     </row>
-    <row r="171" spans="1:18" ht="46.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:18" ht="46.5" thickBot="1">
       <c r="A171" s="1"/>
       <c r="B171" s="9" t="s">
         <v>717</v>
@@ -12492,7 +12510,7 @@
       <c r="Q171" s="1"/>
       <c r="R171" s="1"/>
     </row>
-    <row r="172" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:18" ht="18">
       <c r="A172" s="1"/>
       <c r="B172" s="9" t="s">
         <v>717</v>
@@ -12528,7 +12546,7 @@
       <c r="Q172" s="1"/>
       <c r="R172" s="1"/>
     </row>
-    <row r="173" spans="1:18" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:18" s="24" customFormat="1" ht="18">
       <c r="B173" s="70" t="s">
         <v>717</v>
       </c>
@@ -12556,7 +12574,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="174" spans="1:18" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:18" s="24" customFormat="1" ht="18">
       <c r="B174" s="70"/>
       <c r="C174" s="9"/>
       <c r="D174" s="69"/>
@@ -12568,7 +12586,7 @@
       <c r="J174" s="9"/>
       <c r="K174" s="11"/>
     </row>
-    <row r="175" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:18" ht="18.75">
       <c r="B175" s="72"/>
       <c r="C175" s="72"/>
       <c r="D175" s="72"/>
@@ -12580,7 +12598,7 @@
       <c r="J175" s="72"/>
       <c r="K175" s="73"/>
     </row>
-    <row r="176" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:18" ht="18.75">
       <c r="B176" s="72"/>
       <c r="C176" s="72"/>
       <c r="D176" s="72"/>
@@ -12608,14 +12626,14 @@
   <dimension ref="B2:L269"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="7" ySplit="4" topLeftCell="K5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="4" topLeftCell="J5" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
-      <selection pane="bottomRight" activeCell="K127" sqref="K127"/>
+      <selection pane="bottomRight" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
@@ -12628,7 +12646,7 @@
     <col min="11" max="11" width="77.85546875" style="130" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:11" ht="20.25">
       <c r="B2" s="2" t="s">
         <v>773</v>
       </c>
@@ -12641,7 +12659,7 @@
       <c r="I2" s="5"/>
       <c r="J2" s="3"/>
     </row>
-    <row r="4" spans="2:11" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="45.75">
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -12673,7 +12691,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" ht="27" customHeight="1">
       <c r="B5" s="9"/>
       <c r="C5" s="61" t="s">
         <v>131</v>
@@ -12699,7 +12717,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:11" ht="26.25">
       <c r="B6" s="9"/>
       <c r="C6" s="61" t="s">
         <v>131</v>
@@ -12725,7 +12743,7 @@
         <v>1626</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" ht="30">
       <c r="B7" s="9"/>
       <c r="C7" s="61" t="s">
         <v>131</v>
@@ -12753,7 +12771,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" ht="30">
       <c r="B8" s="9"/>
       <c r="C8" s="61" t="s">
         <v>131</v>
@@ -12777,7 +12795,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" ht="30">
       <c r="B9" s="9" t="s">
         <v>148</v>
       </c>
@@ -12807,7 +12825,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" ht="30">
       <c r="B10" s="9"/>
       <c r="C10" s="61" t="s">
         <v>148</v>
@@ -12835,7 +12853,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" ht="30.75">
       <c r="B11" s="9"/>
       <c r="C11" s="61" t="s">
         <v>148</v>
@@ -12863,7 +12881,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" ht="18">
       <c r="B12" s="9"/>
       <c r="C12" s="61" t="s">
         <v>148</v>
@@ -12891,7 +12909,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="13" spans="2:11" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" ht="45.75">
       <c r="B13" s="9"/>
       <c r="C13" s="61" t="s">
         <v>148</v>
@@ -12921,7 +12939,7 @@
         <v>1625</v>
       </c>
     </row>
-    <row r="14" spans="2:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" ht="20.45" customHeight="1">
       <c r="B14" s="9" t="s">
         <v>148</v>
       </c>
@@ -12951,7 +12969,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="15" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" ht="30">
       <c r="B15" s="9" t="s">
         <v>148</v>
       </c>
@@ -12981,7 +12999,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="16" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:11" ht="26.25">
       <c r="B16" s="9"/>
       <c r="C16" s="9" t="s">
         <v>148</v>
@@ -13009,7 +13027,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" ht="30.75">
       <c r="B17" s="9"/>
       <c r="C17" s="61" t="s">
         <v>148</v>
@@ -13037,7 +13055,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="18" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" ht="18">
       <c r="B18" s="9"/>
       <c r="C18" s="9" t="s">
         <v>148</v>
@@ -13065,7 +13083,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="19" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" ht="30">
       <c r="B19" s="9" t="s">
         <v>148</v>
       </c>
@@ -13095,7 +13113,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:11" ht="26.25">
       <c r="B20" s="25"/>
       <c r="C20" s="66" t="s">
         <v>148</v>
@@ -13121,7 +13139,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="21" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" ht="30">
       <c r="B21" s="9"/>
       <c r="C21" s="61" t="s">
         <v>148</v>
@@ -13149,7 +13167,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="22" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" ht="30">
       <c r="B22" s="9" t="s">
         <v>148</v>
       </c>
@@ -13179,7 +13197,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="23" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" ht="30">
       <c r="B23" s="9"/>
       <c r="C23" s="61" t="s">
         <v>148</v>
@@ -13207,7 +13225,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="24" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" ht="18">
       <c r="B24" s="9"/>
       <c r="C24" s="9" t="s">
         <v>148</v>
@@ -13235,7 +13253,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="25" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" ht="30">
       <c r="B25" s="9" t="s">
         <v>148</v>
       </c>
@@ -13265,7 +13283,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="26" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" ht="30">
       <c r="B26" s="15"/>
       <c r="C26" s="15" t="s">
         <v>148</v>
@@ -13293,7 +13311,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="27" spans="2:11" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" ht="30.75">
       <c r="B27" s="15"/>
       <c r="C27" s="62" t="s">
         <v>148</v>
@@ -13323,7 +13341,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="28" spans="2:11" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" ht="30.75">
       <c r="B28" s="15"/>
       <c r="C28" s="62" t="s">
         <v>148</v>
@@ -13353,7 +13371,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="29" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" ht="18">
       <c r="B29" s="15"/>
       <c r="C29" s="15" t="s">
         <v>148</v>
@@ -13377,7 +13395,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="30" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" ht="30">
       <c r="B30" s="15"/>
       <c r="C30" s="62" t="s">
         <v>1620</v>
@@ -13403,7 +13421,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="31" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" ht="30">
       <c r="B31" s="15"/>
       <c r="C31" s="62" t="s">
         <v>1620</v>
@@ -13427,7 +13445,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="32" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" ht="18">
       <c r="B32" s="15"/>
       <c r="C32" s="61" t="s">
         <v>1620</v>
@@ -13455,7 +13473,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="33" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11" ht="30">
       <c r="B33" s="15"/>
       <c r="C33" s="61" t="s">
         <v>1620</v>
@@ -13479,7 +13497,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="34" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11" ht="18">
       <c r="B34" s="15"/>
       <c r="C34" s="61" t="s">
         <v>1620</v>
@@ -13503,7 +13521,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="35" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" ht="30">
       <c r="B35" s="15"/>
       <c r="C35" s="9" t="s">
         <v>789</v>
@@ -13531,7 +13549,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="36" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11" ht="30">
       <c r="B36" s="15" t="s">
         <v>1457</v>
       </c>
@@ -13561,7 +13579,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="37" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11" ht="30">
       <c r="B37" s="9"/>
       <c r="C37" s="61" t="s">
         <v>789</v>
@@ -13589,7 +13607,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="38" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11" ht="18">
       <c r="B38" s="9"/>
       <c r="C38" s="66" t="s">
         <v>789</v>
@@ -13615,7 +13633,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="39" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:11" ht="18">
       <c r="B39" s="9"/>
       <c r="C39" s="66" t="s">
         <v>789</v>
@@ -13641,7 +13659,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="40" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:11" ht="18">
       <c r="B40" s="9"/>
       <c r="C40" s="61" t="s">
         <v>789</v>
@@ -13669,7 +13687,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="41" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:11" ht="30">
       <c r="B41" s="9" t="s">
         <v>789</v>
       </c>
@@ -13697,7 +13715,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="42" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="42" spans="2:11" ht="26.25">
       <c r="B42" s="9"/>
       <c r="C42" s="61" t="s">
         <v>789</v>
@@ -13721,7 +13739,7 @@
         <v>1628</v>
       </c>
     </row>
-    <row r="43" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="43" spans="2:11" ht="26.25">
       <c r="B43" s="9"/>
       <c r="C43" s="61" t="s">
         <v>789</v>
@@ -13745,7 +13763,7 @@
         <v>1629</v>
       </c>
     </row>
-    <row r="44" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:11" ht="18">
       <c r="B44" s="9"/>
       <c r="C44" s="61" t="s">
         <v>1377</v>
@@ -13771,7 +13789,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="45" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:11" ht="18">
       <c r="B45" s="9"/>
       <c r="C45" s="61" t="s">
         <v>1377</v>
@@ -13799,7 +13817,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="46" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:11" ht="18">
       <c r="B46" s="9"/>
       <c r="C46" s="61" t="s">
         <v>1377</v>
@@ -13827,7 +13845,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="47" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:11" ht="30">
       <c r="B47" s="9"/>
       <c r="C47" s="61" t="s">
         <v>1377</v>
@@ -13853,7 +13871,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="48" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:11" ht="30">
       <c r="B48" s="8" t="s">
         <v>15</v>
       </c>
@@ -13883,7 +13901,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="49" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B49" s="8" t="s">
         <v>15</v>
       </c>
@@ -13913,7 +13931,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="50" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B50" s="8" t="s">
         <v>15</v>
       </c>
@@ -13943,7 +13961,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="51" spans="2:11" s="1" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:11" s="1" customFormat="1" ht="30.75">
       <c r="B51" s="8" t="s">
         <v>15</v>
       </c>
@@ -13973,7 +13991,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="52" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B52" s="8" t="s">
         <v>15</v>
       </c>
@@ -14003,7 +14021,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="53" spans="2:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11" s="1" customFormat="1" ht="45">
       <c r="B53" s="8" t="s">
         <v>15</v>
       </c>
@@ -14033,7 +14051,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="54" spans="2:11" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:11" s="24" customFormat="1" ht="18">
       <c r="B54" s="9" t="s">
         <v>15</v>
       </c>
@@ -14061,7 +14079,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="55" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:11" s="24" customFormat="1" ht="30">
       <c r="B55" s="9" t="s">
         <v>15</v>
       </c>
@@ -14089,7 +14107,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="56" spans="2:11" s="24" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="56" spans="2:11" s="24" customFormat="1" ht="26.25">
       <c r="B56" s="9" t="s">
         <v>15</v>
       </c>
@@ -14117,7 +14135,7 @@
         <v>1630</v>
       </c>
     </row>
-    <row r="57" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:11" s="24" customFormat="1" ht="30">
       <c r="B57" s="9"/>
       <c r="C57" s="61" t="s">
         <v>1127</v>
@@ -14141,7 +14159,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="58" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:11" s="24" customFormat="1" ht="30">
       <c r="B58" s="9"/>
       <c r="C58" s="61" t="s">
         <v>1127</v>
@@ -14165,7 +14183,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="59" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:11" s="24" customFormat="1" ht="30">
       <c r="B59" s="9"/>
       <c r="C59" s="61" t="s">
         <v>1127</v>
@@ -14189,7 +14207,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="60" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:11" s="24" customFormat="1" ht="30">
       <c r="B60" s="9"/>
       <c r="C60" s="61" t="s">
         <v>1127</v>
@@ -14213,7 +14231,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="61" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:11" s="24" customFormat="1" ht="30">
       <c r="B61" s="9"/>
       <c r="C61" s="61" t="s">
         <v>1127</v>
@@ -14237,7 +14255,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="62" spans="2:11" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:11" s="24" customFormat="1" ht="18">
       <c r="B62" s="9"/>
       <c r="C62" s="61" t="s">
         <v>1127</v>
@@ -14263,7 +14281,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="63" spans="2:11" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:11" s="24" customFormat="1" ht="18">
       <c r="B63" s="9"/>
       <c r="C63" s="61" t="s">
         <v>1127</v>
@@ -14289,7 +14307,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="64" spans="2:11" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:11" s="24" customFormat="1" ht="18">
       <c r="B64" s="9"/>
       <c r="C64" s="61" t="s">
         <v>1127</v>
@@ -14313,7 +14331,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="65" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:11" ht="30">
       <c r="B65" s="9"/>
       <c r="C65" s="61" t="s">
         <v>1127</v>
@@ -14341,7 +14359,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="66" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:11" ht="18">
       <c r="B66" s="9"/>
       <c r="C66" s="61" t="s">
         <v>1127</v>
@@ -14367,7 +14385,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="67" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:11" ht="45">
       <c r="B67" s="9"/>
       <c r="C67" s="61" t="s">
         <v>1376</v>
@@ -14395,7 +14413,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="68" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:11" ht="45">
       <c r="B68" s="9"/>
       <c r="C68" s="61" t="s">
         <v>1331</v>
@@ -14423,7 +14441,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="69" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:11" ht="30">
       <c r="B69" s="25"/>
       <c r="C69" s="61" t="s">
         <v>1331</v>
@@ -14449,7 +14467,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="70" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:11" ht="30">
       <c r="B70" s="25"/>
       <c r="C70" s="9" t="s">
         <v>1331</v>
@@ -14477,7 +14495,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="71" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:11" ht="30">
       <c r="B71" s="9"/>
       <c r="C71" s="61" t="s">
         <v>1331</v>
@@ -14503,7 +14521,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="72" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:11" ht="30">
       <c r="B72" s="25"/>
       <c r="C72" s="60" t="s">
         <v>1331</v>
@@ -14531,7 +14549,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="73" spans="2:11" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:11" s="24" customFormat="1" ht="30">
       <c r="B73" s="9"/>
       <c r="C73" s="61" t="s">
         <v>139</v>
@@ -14559,7 +14577,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="74" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:11" ht="30">
       <c r="B74" s="9"/>
       <c r="C74" s="61" t="s">
         <v>139</v>
@@ -14587,7 +14605,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="75" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:11" ht="18">
       <c r="B75" s="9" t="s">
         <v>139</v>
       </c>
@@ -14617,7 +14635,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="76" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:11" ht="18">
       <c r="B76" s="9" t="s">
         <v>139</v>
       </c>
@@ -14645,7 +14663,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="77" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:11" ht="30">
       <c r="B77" s="9"/>
       <c r="C77" s="9" t="s">
         <v>1310</v>
@@ -14673,7 +14691,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="78" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:11" ht="30">
       <c r="B78" s="9"/>
       <c r="C78" s="9" t="s">
         <v>1310</v>
@@ -14701,7 +14719,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="79" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:11" ht="18">
       <c r="B79" s="9"/>
       <c r="C79" s="61" t="s">
         <v>1310</v>
@@ -14729,7 +14747,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="80" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:11" ht="30">
       <c r="B80" s="9"/>
       <c r="C80" s="61" t="s">
         <v>1617</v>
@@ -14755,7 +14773,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="81" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:11" ht="30">
       <c r="B81" s="9"/>
       <c r="C81" s="61" t="s">
         <v>1617</v>
@@ -14781,7 +14799,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="82" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:11" ht="30">
       <c r="B82" s="9"/>
       <c r="C82" s="9" t="s">
         <v>7</v>
@@ -14809,7 +14827,7 @@
         <v>1694</v>
       </c>
     </row>
-    <row r="83" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:11" ht="30">
       <c r="B83" s="9"/>
       <c r="C83" s="9" t="s">
         <v>7</v>
@@ -14837,7 +14855,7 @@
         <v>1693</v>
       </c>
     </row>
-    <row r="84" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:11" ht="18">
       <c r="B84" s="25"/>
       <c r="C84" s="9" t="s">
         <v>7</v>
@@ -14865,7 +14883,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="85" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:11" ht="30">
       <c r="B85" s="9"/>
       <c r="C85" s="66" t="s">
         <v>7</v>
@@ -14891,7 +14909,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="86" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:11" ht="30">
       <c r="B86" s="9"/>
       <c r="C86" s="61" t="s">
         <v>7</v>
@@ -14917,7 +14935,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="87" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:11" ht="30">
       <c r="B87" s="9"/>
       <c r="C87" s="61" t="s">
         <v>7</v>
@@ -14943,7 +14961,7 @@
         <v>1695</v>
       </c>
     </row>
-    <row r="88" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:11" ht="30">
       <c r="B88" s="9"/>
       <c r="C88" s="61" t="s">
         <v>7</v>
@@ -14969,7 +14987,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="89" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:11" ht="30">
       <c r="B89" s="9" t="s">
         <v>60</v>
       </c>
@@ -14999,7 +15017,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="90" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:11" ht="30">
       <c r="B90" s="9"/>
       <c r="C90" s="61" t="s">
         <v>7</v>
@@ -15025,7 +15043,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="91" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:11" ht="30">
       <c r="B91" s="9"/>
       <c r="C91" s="61" t="s">
         <v>7</v>
@@ -15053,7 +15071,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="92" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:11" ht="30">
       <c r="B92" s="9"/>
       <c r="C92" s="61" t="s">
         <v>7</v>
@@ -15079,7 +15097,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="93" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:11" ht="18">
       <c r="B93" s="9"/>
       <c r="C93" s="61" t="s">
         <v>7</v>
@@ -15105,7 +15123,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="94" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:11" ht="18">
       <c r="B94" s="25"/>
       <c r="C94" s="9" t="s">
         <v>7</v>
@@ -15133,7 +15151,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="95" spans="2:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:11" ht="45">
       <c r="B95" s="9"/>
       <c r="C95" s="61" t="s">
         <v>7</v>
@@ -15159,7 +15177,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="96" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:11" ht="18">
       <c r="B96" s="25" t="s">
         <v>710</v>
       </c>
@@ -15189,7 +15207,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="97" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:11" ht="18">
       <c r="B97" s="9" t="s">
         <v>148</v>
       </c>
@@ -15217,7 +15235,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="98" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:11" ht="30">
       <c r="B98" s="9" t="s">
         <v>19</v>
       </c>
@@ -15245,7 +15263,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="99" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:11" ht="18">
       <c r="B99" s="9" t="s">
         <v>710</v>
       </c>
@@ -15273,7 +15291,7 @@
         <v>1691</v>
       </c>
     </row>
-    <row r="100" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:11" ht="18">
       <c r="B100" s="25"/>
       <c r="C100" s="9" t="s">
         <v>7</v>
@@ -15301,7 +15319,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="101" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:11" ht="18">
       <c r="B101" s="25"/>
       <c r="C101" s="9" t="s">
         <v>7</v>
@@ -15327,7 +15345,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="102" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:11" ht="30">
       <c r="B102" s="25"/>
       <c r="C102" s="9" t="s">
         <v>7</v>
@@ -15353,7 +15371,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="103" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:11" ht="18">
       <c r="B103" s="25" t="s">
         <v>710</v>
       </c>
@@ -15383,7 +15401,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="104" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:11" ht="18">
       <c r="B104" s="25" t="s">
         <v>710</v>
       </c>
@@ -15411,7 +15429,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="105" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B105" s="9" t="s">
         <v>711</v>
       </c>
@@ -15441,7 +15459,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="106" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B106" s="9" t="s">
         <v>148</v>
       </c>
@@ -15467,7 +15485,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="107" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="107" spans="2:11" s="1" customFormat="1" ht="26.25">
       <c r="B107" s="9"/>
       <c r="C107" s="9" t="s">
         <v>7</v>
@@ -15495,7 +15513,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="108" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B108" s="9"/>
       <c r="C108" s="61" t="s">
         <v>7</v>
@@ -15519,7 +15537,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="109" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B109" s="9"/>
       <c r="C109" s="61" t="s">
         <v>7</v>
@@ -15543,7 +15561,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="110" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B110" s="9"/>
       <c r="C110" s="61" t="s">
         <v>7</v>
@@ -15567,7 +15585,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="111" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B111" s="9"/>
       <c r="C111" s="9" t="s">
         <v>1255</v>
@@ -15595,7 +15613,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="112" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B112" s="9"/>
       <c r="C112" s="9" t="s">
         <v>1255</v>
@@ -15623,7 +15641,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="113" spans="2:12" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:12" s="1" customFormat="1" ht="18">
       <c r="B113" s="25"/>
       <c r="C113" s="9" t="s">
         <v>1255</v>
@@ -15651,7 +15669,7 @@
         <v>1696</v>
       </c>
     </row>
-    <row r="114" spans="2:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:12" s="1" customFormat="1" ht="45">
       <c r="B114" s="9"/>
       <c r="C114" s="61" t="s">
         <v>1546</v>
@@ -15677,7 +15695,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="115" spans="2:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:12" s="1" customFormat="1" ht="30">
       <c r="B115" s="9"/>
       <c r="C115" s="61" t="s">
         <v>1546</v>
@@ -15705,7 +15723,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="116" spans="2:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:12" s="1" customFormat="1" ht="30">
       <c r="B116" s="9"/>
       <c r="C116" s="61" t="s">
         <v>1546</v>
@@ -15731,7 +15749,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="117" spans="2:12" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:12" s="1" customFormat="1" ht="18">
       <c r="B117" s="9"/>
       <c r="C117" s="61" t="s">
         <v>1546</v>
@@ -15757,7 +15775,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="118" spans="2:12" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:12" s="1" customFormat="1" ht="18">
       <c r="B118" s="9"/>
       <c r="C118" s="61" t="s">
         <v>1546</v>
@@ -15783,7 +15801,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="119" spans="2:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:12" s="1" customFormat="1" ht="45">
       <c r="B119" s="9"/>
       <c r="C119" s="61" t="s">
         <v>1546</v>
@@ -15809,7 +15827,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="120" spans="2:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:12" s="1" customFormat="1" ht="30">
       <c r="B120" s="9"/>
       <c r="C120" s="61" t="s">
         <v>1546</v>
@@ -15835,7 +15853,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="121" spans="2:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:12" s="1" customFormat="1" ht="30">
       <c r="B121" s="9"/>
       <c r="C121" s="61" t="s">
         <v>1546</v>
@@ -15861,7 +15879,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="122" spans="2:12" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="122" spans="2:12" s="1" customFormat="1" ht="26.25">
       <c r="B122" s="9"/>
       <c r="C122" s="61" t="s">
         <v>1546</v>
@@ -15887,7 +15905,7 @@
         <v>1631</v>
       </c>
     </row>
-    <row r="123" spans="2:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:12" s="1" customFormat="1" ht="60">
       <c r="B123" s="9"/>
       <c r="C123" s="61" t="s">
         <v>1546</v>
@@ -15913,7 +15931,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="124" spans="2:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:12" s="1" customFormat="1" ht="30">
       <c r="B124" s="9"/>
       <c r="C124" s="61" t="s">
         <v>1546</v>
@@ -15939,7 +15957,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="125" spans="2:12" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:12" s="1" customFormat="1" ht="18">
       <c r="B125" s="9"/>
       <c r="C125" s="61" t="s">
         <v>1546</v>
@@ -15965,7 +15983,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="126" spans="2:12" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:12" s="1" customFormat="1" ht="18">
       <c r="B126" s="9"/>
       <c r="C126" s="61" t="s">
         <v>1546</v>
@@ -15993,7 +16011,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="127" spans="2:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:12" s="1" customFormat="1" ht="60">
       <c r="B127" s="9"/>
       <c r="C127" s="61" t="s">
         <v>1546</v>
@@ -16021,7 +16039,7 @@
         <v>1699</v>
       </c>
     </row>
-    <row r="128" spans="2:12" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:12" s="1" customFormat="1" ht="18">
       <c r="B128" s="9"/>
       <c r="C128" s="61" t="s">
         <v>1546</v>
@@ -16048,7 +16066,7 @@
         <v>1698</v>
       </c>
     </row>
-    <row r="129" spans="2:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:11" s="1" customFormat="1" ht="45">
       <c r="B129" s="58"/>
       <c r="C129" s="61" t="s">
         <v>1546</v>
@@ -16074,7 +16092,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="130" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B130" s="9"/>
       <c r="C130" s="61" t="s">
         <v>1546</v>
@@ -16100,7 +16118,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="131" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B131" s="9"/>
       <c r="C131" s="61" t="s">
         <v>1546</v>
@@ -16126,7 +16144,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="132" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B132" s="9"/>
       <c r="C132" s="61" t="s">
         <v>1546</v>
@@ -16152,7 +16170,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="133" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B133" s="9"/>
       <c r="C133" s="61" t="s">
         <v>1546</v>
@@ -16178,7 +16196,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="134" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B134" s="9"/>
       <c r="C134" s="61" t="s">
         <v>1546</v>
@@ -16204,7 +16222,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="135" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B135" s="9"/>
       <c r="C135" s="61" t="s">
         <v>1546</v>
@@ -16230,7 +16248,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="136" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B136" s="9"/>
       <c r="C136" s="61" t="s">
         <v>1546</v>
@@ -16254,7 +16272,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="137" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B137" s="9"/>
       <c r="C137" s="61" t="s">
         <v>1546</v>
@@ -16282,7 +16300,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="138" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B138" s="9"/>
       <c r="C138" s="61" t="s">
         <v>1546</v>
@@ -16308,7 +16326,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="139" spans="2:11" s="59" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:11" s="59" customFormat="1" ht="18">
       <c r="B139" s="9"/>
       <c r="C139" s="61" t="s">
         <v>1546</v>
@@ -16332,7 +16350,7 @@
         <v>1701</v>
       </c>
     </row>
-    <row r="140" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B140" s="9"/>
       <c r="C140" s="61" t="s">
         <v>1546</v>
@@ -16356,7 +16374,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="141" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B141" s="8" t="s">
         <v>19</v>
       </c>
@@ -16384,7 +16402,7 @@
       </c>
       <c r="K141" s="85"/>
     </row>
-    <row r="142" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B142" s="8" t="s">
         <v>19</v>
       </c>
@@ -16414,7 +16432,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="143" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B143" s="8" t="s">
         <v>19</v>
       </c>
@@ -16444,7 +16462,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="144" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B144" s="8" t="s">
         <v>19</v>
       </c>
@@ -16474,7 +16492,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="145" spans="2:11" s="1" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:11" s="1" customFormat="1" ht="30.75">
       <c r="B145" s="8" t="s">
         <v>19</v>
       </c>
@@ -16504,7 +16522,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="146" spans="2:11" s="1" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:11" s="1" customFormat="1" ht="30.75">
       <c r="B146" s="9"/>
       <c r="C146" s="66" t="s">
         <v>60</v>
@@ -16532,7 +16550,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="147" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B147" s="9"/>
       <c r="C147" s="9" t="s">
         <v>60</v>
@@ -16560,7 +16578,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="148" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B148" s="9"/>
       <c r="C148" s="61" t="s">
         <v>60</v>
@@ -16588,7 +16606,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="149" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B149" s="9"/>
       <c r="C149" s="9" t="s">
         <v>60</v>
@@ -16616,7 +16634,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="150" spans="2:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:11" s="1" customFormat="1" ht="45">
       <c r="B150" s="9"/>
       <c r="C150" s="61" t="s">
         <v>60</v>
@@ -16642,7 +16660,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="151" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B151" s="9" t="s">
         <v>7</v>
       </c>
@@ -16672,7 +16690,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="152" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B152" s="9" t="s">
         <v>711</v>
       </c>
@@ -16700,7 +16718,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="153" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B153" s="9" t="s">
         <v>711</v>
       </c>
@@ -16728,7 +16746,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="154" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B154" s="9"/>
       <c r="C154" s="63" t="s">
         <v>60</v>
@@ -16754,7 +16772,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="155" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B155" s="9" t="s">
         <v>1381</v>
       </c>
@@ -16782,7 +16800,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="156" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="156" spans="2:11" s="1" customFormat="1" ht="26.25">
       <c r="B156" s="9"/>
       <c r="C156" s="66" t="s">
         <v>717</v>
@@ -16808,7 +16826,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="157" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B157" s="9"/>
       <c r="C157" s="61" t="s">
         <v>717</v>
@@ -16836,7 +16854,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="158" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B158" s="9"/>
       <c r="C158" s="61" t="s">
         <v>717</v>
@@ -16864,7 +16882,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="159" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B159" s="45"/>
       <c r="C159" s="61" t="s">
         <v>717</v>
@@ -16892,7 +16910,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="160" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B160" s="9"/>
       <c r="C160" s="9" t="s">
         <v>717</v>
@@ -16920,7 +16938,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="161" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B161" s="9"/>
       <c r="C161" s="9" t="s">
         <v>717</v>
@@ -16948,7 +16966,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="162" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B162" s="9"/>
       <c r="C162" s="61" t="s">
         <v>717</v>
@@ -16976,7 +16994,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="163" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B163" s="9"/>
       <c r="C163" s="61" t="s">
         <v>717</v>
@@ -17004,7 +17022,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="164" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B164" s="9" t="s">
         <v>715</v>
       </c>
@@ -17034,7 +17052,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="165" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B165" s="9" t="s">
         <v>715</v>
       </c>
@@ -17064,7 +17082,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="166" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B166" s="9" t="s">
         <v>715</v>
       </c>
@@ -17094,7 +17112,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="167" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B167" s="9"/>
       <c r="C167" s="9" t="s">
         <v>717</v>
@@ -17122,7 +17140,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="168" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B168" s="9"/>
       <c r="C168" s="61" t="s">
         <v>717</v>
@@ -17148,7 +17166,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="169" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B169" s="9"/>
       <c r="C169" s="66" t="s">
         <v>717</v>
@@ -17176,7 +17194,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="170" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="170" spans="2:11" s="1" customFormat="1" ht="26.25">
       <c r="B170" s="45"/>
       <c r="C170" s="61" t="s">
         <v>717</v>
@@ -17202,7 +17220,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="171" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="171" spans="2:11" s="1" customFormat="1" ht="26.25">
       <c r="B171" s="9"/>
       <c r="C171" s="66" t="s">
         <v>717</v>
@@ -17228,7 +17246,7 @@
         <v>1633</v>
       </c>
     </row>
-    <row r="172" spans="2:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:11" s="1" customFormat="1" ht="45">
       <c r="B172" s="9"/>
       <c r="C172" s="9" t="s">
         <v>717</v>
@@ -17254,7 +17272,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="173" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B173" s="9" t="s">
         <v>717</v>
       </c>
@@ -17284,7 +17302,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="174" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B174" s="9" t="s">
         <v>717</v>
       </c>
@@ -17314,7 +17332,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="175" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B175" s="9"/>
       <c r="C175" s="61" t="s">
         <v>717</v>
@@ -17342,7 +17360,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="176" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="176" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B176" s="9"/>
       <c r="C176" s="61" t="s">
         <v>717</v>
@@ -17368,7 +17386,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="177" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="177" spans="2:11" s="1" customFormat="1" ht="26.25">
       <c r="B177" s="9"/>
       <c r="C177" s="66" t="s">
         <v>717</v>
@@ -17394,7 +17412,7 @@
         <v>1634</v>
       </c>
     </row>
-    <row r="178" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B178" s="9"/>
       <c r="C178" s="61" t="s">
         <v>717</v>
@@ -17422,7 +17440,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="179" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B179" s="9"/>
       <c r="C179" s="61" t="s">
         <v>717</v>
@@ -17450,7 +17468,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="180" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="180" spans="2:11" s="1" customFormat="1" ht="26.25">
       <c r="B180" s="9"/>
       <c r="C180" s="61" t="s">
         <v>717</v>
@@ -17478,7 +17496,7 @@
         <v>1635</v>
       </c>
     </row>
-    <row r="181" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B181" s="9"/>
       <c r="C181" s="61" t="s">
         <v>717</v>
@@ -17506,7 +17524,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="182" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="182" spans="2:11" s="1" customFormat="1" ht="26.25">
       <c r="B182" s="9"/>
       <c r="C182" s="61" t="s">
         <v>717</v>
@@ -17534,7 +17552,7 @@
         <v>1636</v>
       </c>
     </row>
-    <row r="183" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B183" s="9"/>
       <c r="C183" s="61" t="s">
         <v>717</v>
@@ -17562,7 +17580,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="184" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="184" spans="2:11" s="1" customFormat="1" ht="26.25">
       <c r="B184" s="9"/>
       <c r="C184" s="61" t="s">
         <v>717</v>
@@ -17590,7 +17608,7 @@
         <v>1637</v>
       </c>
     </row>
-    <row r="185" spans="2:11" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="185" spans="2:11" s="1" customFormat="1" ht="26.25">
       <c r="B185" s="9"/>
       <c r="C185" s="9" t="s">
         <v>60</v>
@@ -17620,7 +17638,7 @@
         <v>1638</v>
       </c>
     </row>
-    <row r="186" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B186" s="9" t="s">
         <v>7</v>
       </c>
@@ -17646,7 +17664,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="187" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B187" s="9" t="s">
         <v>148</v>
       </c>
@@ -17672,7 +17690,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="188" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B188" s="9" t="s">
         <v>148</v>
       </c>
@@ -17698,7 +17716,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="189" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B189" s="9" t="s">
         <v>148</v>
       </c>
@@ -17724,7 +17742,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="190" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B190" s="25"/>
       <c r="C190" s="9" t="s">
         <v>717</v>
@@ -17748,7 +17766,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="191" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B191" s="45"/>
       <c r="C191" s="9" t="s">
         <v>717</v>
@@ -17772,7 +17790,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="192" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B192" s="9"/>
       <c r="C192" s="9" t="s">
         <v>717</v>
@@ -17796,7 +17814,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="193" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B193" s="9"/>
       <c r="C193" s="9" t="s">
         <v>717</v>
@@ -17820,7 +17838,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="194" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B194" s="9"/>
       <c r="C194" s="9" t="s">
         <v>717</v>
@@ -17844,7 +17862,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="195" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B195" s="9"/>
       <c r="C195" s="61" t="s">
         <v>717</v>
@@ -17868,7 +17886,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="196" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B196" s="9"/>
       <c r="C196" s="61" t="s">
         <v>717</v>
@@ -17892,7 +17910,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="197" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B197" s="9"/>
       <c r="C197" s="61" t="s">
         <v>717</v>
@@ -17916,7 +17934,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="198" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B198" s="9"/>
       <c r="C198" s="61" t="s">
         <v>717</v>
@@ -17940,7 +17958,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="199" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B199" s="9" t="s">
         <v>7</v>
       </c>
@@ -17970,7 +17988,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="200" spans="2:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:11" s="1" customFormat="1" ht="18">
       <c r="B200" s="9" t="s">
         <v>7</v>
       </c>
@@ -18000,7 +18018,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="201" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B201" s="9"/>
       <c r="C201" s="61" t="s">
         <v>1619</v>
@@ -18024,7 +18042,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="202" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B202" s="9"/>
       <c r="C202" s="61" t="s">
         <v>1619</v>
@@ -18048,7 +18066,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="203" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B203" s="9"/>
       <c r="C203" s="61" t="s">
         <v>1619</v>
@@ -18072,7 +18090,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="204" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B204" s="9"/>
       <c r="C204" s="61" t="s">
         <v>1619</v>
@@ -18096,7 +18114,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="205" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B205" s="9"/>
       <c r="C205" s="61" t="s">
         <v>1619</v>
@@ -18120,7 +18138,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="206" spans="2:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:11" s="1" customFormat="1" ht="30">
       <c r="B206" s="9"/>
       <c r="C206" s="61" t="s">
         <v>1619</v>
@@ -18144,7 +18162,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="207" spans="2:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:11" ht="18">
       <c r="B207" s="69"/>
       <c r="C207" s="84" t="s">
         <v>1619</v>
@@ -18168,7 +18186,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="208" spans="2:11" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:11" s="24" customFormat="1" ht="18">
       <c r="B208" s="9"/>
       <c r="C208" s="61" t="s">
         <v>1619</v>
@@ -18192,7 +18210,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="209" spans="2:11" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:11" s="24" customFormat="1" ht="18">
       <c r="B209" s="45"/>
       <c r="C209" s="45"/>
       <c r="D209" s="45"/>
@@ -18204,7 +18222,7 @@
       <c r="J209" s="45"/>
       <c r="K209" s="54"/>
     </row>
-    <row r="210" spans="2:11" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:11" s="24" customFormat="1" ht="18">
       <c r="B210" s="25"/>
       <c r="C210" s="25"/>
       <c r="D210" s="25"/>
@@ -18216,7 +18234,7 @@
       <c r="J210" s="25"/>
       <c r="K210" s="54"/>
     </row>
-    <row r="211" spans="2:11" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:11" s="24" customFormat="1" ht="18">
       <c r="B211" s="25"/>
       <c r="C211" s="25"/>
       <c r="D211" s="25"/>
@@ -18228,7 +18246,7 @@
       <c r="J211" s="25"/>
       <c r="K211" s="54"/>
     </row>
-    <row r="212" spans="2:11" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:11" s="24" customFormat="1" ht="18">
       <c r="B212" s="25"/>
       <c r="C212" s="25"/>
       <c r="D212" s="25"/>
@@ -18240,7 +18258,7 @@
       <c r="J212" s="25"/>
       <c r="K212" s="54"/>
     </row>
-    <row r="213" spans="2:11" s="24" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:11" s="24" customFormat="1" ht="18">
       <c r="B213" s="25"/>
       <c r="C213" s="25"/>
       <c r="D213" s="25"/>
@@ -18252,7 +18270,7 @@
       <c r="J213" s="25"/>
       <c r="K213" s="54"/>
     </row>
-    <row r="214" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:11">
       <c r="B214" s="45"/>
       <c r="C214" s="45"/>
       <c r="D214" s="45"/>
@@ -18264,7 +18282,7 @@
       <c r="J214" s="45"/>
       <c r="K214" s="54"/>
     </row>
-    <row r="215" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:11">
       <c r="B215" s="45"/>
       <c r="C215" s="45"/>
       <c r="D215" s="45"/>
@@ -18276,7 +18294,7 @@
       <c r="J215" s="45"/>
       <c r="K215" s="54"/>
     </row>
-    <row r="216" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:11">
       <c r="B216" s="45"/>
       <c r="C216" s="45"/>
       <c r="D216" s="45"/>
@@ -18288,7 +18306,7 @@
       <c r="J216" s="45"/>
       <c r="K216" s="54"/>
     </row>
-    <row r="217" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:11">
       <c r="B217" s="45"/>
       <c r="C217" s="45"/>
       <c r="D217" s="45"/>
@@ -18300,7 +18318,7 @@
       <c r="J217" s="45"/>
       <c r="K217" s="54"/>
     </row>
-    <row r="218" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:11">
       <c r="B218" s="45"/>
       <c r="C218" s="45"/>
       <c r="D218" s="45"/>
@@ -18312,7 +18330,7 @@
       <c r="J218" s="45"/>
       <c r="K218" s="54"/>
     </row>
-    <row r="219" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:11">
       <c r="B219" s="45"/>
       <c r="C219" s="45"/>
       <c r="D219" s="45"/>
@@ -18324,7 +18342,7 @@
       <c r="J219" s="45"/>
       <c r="K219" s="54"/>
     </row>
-    <row r="220" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:11">
       <c r="B220" s="45"/>
       <c r="C220" s="45"/>
       <c r="D220" s="45"/>
@@ -18336,7 +18354,7 @@
       <c r="J220" s="45"/>
       <c r="K220" s="54"/>
     </row>
-    <row r="221" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:11">
       <c r="B221" s="45"/>
       <c r="C221" s="45"/>
       <c r="D221" s="45"/>
@@ -18348,7 +18366,7 @@
       <c r="J221" s="45"/>
       <c r="K221" s="54"/>
     </row>
-    <row r="222" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:11">
       <c r="B222" s="45"/>
       <c r="C222" s="45"/>
       <c r="D222" s="45"/>
@@ -18360,7 +18378,7 @@
       <c r="J222" s="45"/>
       <c r="K222" s="54"/>
     </row>
-    <row r="223" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:11">
       <c r="B223" s="45"/>
       <c r="C223" s="45"/>
       <c r="D223" s="45"/>
@@ -18372,7 +18390,7 @@
       <c r="J223" s="45"/>
       <c r="K223" s="54"/>
     </row>
-    <row r="224" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:11">
       <c r="B224" s="45"/>
       <c r="C224" s="45"/>
       <c r="D224" s="45"/>
@@ -18384,7 +18402,7 @@
       <c r="J224" s="45"/>
       <c r="K224" s="54"/>
     </row>
-    <row r="225" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:11">
       <c r="B225" s="45"/>
       <c r="C225" s="45"/>
       <c r="D225" s="45"/>
@@ -18396,7 +18414,7 @@
       <c r="J225" s="45"/>
       <c r="K225" s="54"/>
     </row>
-    <row r="226" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:11">
       <c r="B226" s="45"/>
       <c r="C226" s="45"/>
       <c r="D226" s="45"/>
@@ -18408,7 +18426,7 @@
       <c r="J226" s="45"/>
       <c r="K226" s="54"/>
     </row>
-    <row r="227" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:11">
       <c r="B227" s="45"/>
       <c r="C227" s="45"/>
       <c r="D227" s="45"/>
@@ -18420,7 +18438,7 @@
       <c r="J227" s="45"/>
       <c r="K227" s="54"/>
     </row>
-    <row r="228" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:11">
       <c r="B228" s="45"/>
       <c r="C228" s="45"/>
       <c r="D228" s="45"/>
@@ -18432,7 +18450,7 @@
       <c r="J228" s="45"/>
       <c r="K228" s="54"/>
     </row>
-    <row r="229" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:11">
       <c r="B229" s="45"/>
       <c r="C229" s="45"/>
       <c r="D229" s="45"/>
@@ -18444,7 +18462,7 @@
       <c r="J229" s="45"/>
       <c r="K229" s="54"/>
     </row>
-    <row r="230" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:11">
       <c r="B230" s="45"/>
       <c r="C230" s="45"/>
       <c r="D230" s="45"/>
@@ -18456,7 +18474,7 @@
       <c r="J230" s="45"/>
       <c r="K230" s="54"/>
     </row>
-    <row r="231" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="231" spans="2:11">
       <c r="B231" s="45"/>
       <c r="C231" s="45"/>
       <c r="D231" s="45"/>
@@ -18468,7 +18486,7 @@
       <c r="J231" s="45"/>
       <c r="K231" s="54"/>
     </row>
-    <row r="232" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="232" spans="2:11">
       <c r="B232" s="45"/>
       <c r="C232" s="45"/>
       <c r="D232" s="45"/>
@@ -18480,7 +18498,7 @@
       <c r="J232" s="45"/>
       <c r="K232" s="54"/>
     </row>
-    <row r="233" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="233" spans="2:11">
       <c r="B233" s="45"/>
       <c r="C233" s="45"/>
       <c r="D233" s="45"/>
@@ -18492,7 +18510,7 @@
       <c r="J233" s="45"/>
       <c r="K233" s="54"/>
     </row>
-    <row r="234" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:11">
       <c r="B234" s="45"/>
       <c r="C234" s="45"/>
       <c r="D234" s="45"/>
@@ -18504,7 +18522,7 @@
       <c r="J234" s="45"/>
       <c r="K234" s="54"/>
     </row>
-    <row r="235" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="235" spans="2:11">
       <c r="B235" s="45"/>
       <c r="C235" s="45"/>
       <c r="D235" s="45"/>
@@ -18516,7 +18534,7 @@
       <c r="J235" s="45"/>
       <c r="K235" s="54"/>
     </row>
-    <row r="236" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:11">
       <c r="B236" s="45"/>
       <c r="C236" s="45"/>
       <c r="D236" s="45"/>
@@ -18528,7 +18546,7 @@
       <c r="J236" s="45"/>
       <c r="K236" s="54"/>
     </row>
-    <row r="237" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:11">
       <c r="B237" s="45"/>
       <c r="C237" s="45"/>
       <c r="D237" s="45"/>
@@ -18540,7 +18558,7 @@
       <c r="J237" s="45"/>
       <c r="K237" s="54"/>
     </row>
-    <row r="238" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="238" spans="2:11">
       <c r="B238" s="45"/>
       <c r="C238" s="45"/>
       <c r="D238" s="45"/>
@@ -18552,7 +18570,7 @@
       <c r="J238" s="45"/>
       <c r="K238" s="54"/>
     </row>
-    <row r="239" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:11">
       <c r="B239" s="45"/>
       <c r="C239" s="45"/>
       <c r="D239" s="45"/>
@@ -18564,7 +18582,7 @@
       <c r="J239" s="45"/>
       <c r="K239" s="54"/>
     </row>
-    <row r="240" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:11">
       <c r="B240" s="45"/>
       <c r="C240" s="45"/>
       <c r="D240" s="45"/>
@@ -18576,7 +18594,7 @@
       <c r="J240" s="45"/>
       <c r="K240" s="54"/>
     </row>
-    <row r="241" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="241" spans="2:11">
       <c r="B241" s="45"/>
       <c r="C241" s="45"/>
       <c r="D241" s="45"/>
@@ -18588,7 +18606,7 @@
       <c r="J241" s="45"/>
       <c r="K241" s="54"/>
     </row>
-    <row r="242" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="242" spans="2:11">
       <c r="B242" s="45"/>
       <c r="C242" s="45"/>
       <c r="D242" s="45"/>
@@ -18600,7 +18618,7 @@
       <c r="J242" s="45"/>
       <c r="K242" s="54"/>
     </row>
-    <row r="243" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="243" spans="2:11">
       <c r="B243" s="45"/>
       <c r="C243" s="45"/>
       <c r="D243" s="45"/>
@@ -18612,7 +18630,7 @@
       <c r="J243" s="45"/>
       <c r="K243" s="54"/>
     </row>
-    <row r="244" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="244" spans="2:11">
       <c r="B244" s="45"/>
       <c r="C244" s="45"/>
       <c r="D244" s="45"/>
@@ -18624,7 +18642,7 @@
       <c r="J244" s="45"/>
       <c r="K244" s="54"/>
     </row>
-    <row r="245" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="245" spans="2:11">
       <c r="B245" s="45"/>
       <c r="C245" s="45"/>
       <c r="D245" s="45"/>
@@ -18636,7 +18654,7 @@
       <c r="J245" s="45"/>
       <c r="K245" s="54"/>
     </row>
-    <row r="246" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="246" spans="2:11">
       <c r="B246" s="45"/>
       <c r="C246" s="45"/>
       <c r="D246" s="45"/>
@@ -18648,7 +18666,7 @@
       <c r="J246" s="45"/>
       <c r="K246" s="54"/>
     </row>
-    <row r="247" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="247" spans="2:11">
       <c r="B247" s="45"/>
       <c r="C247" s="45"/>
       <c r="D247" s="45"/>
@@ -18660,7 +18678,7 @@
       <c r="J247" s="45"/>
       <c r="K247" s="54"/>
     </row>
-    <row r="248" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="248" spans="2:11">
       <c r="B248" s="45"/>
       <c r="C248" s="45"/>
       <c r="D248" s="45"/>
@@ -18672,7 +18690,7 @@
       <c r="J248" s="45"/>
       <c r="K248" s="54"/>
     </row>
-    <row r="249" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:11">
       <c r="B249" s="45"/>
       <c r="C249" s="45"/>
       <c r="D249" s="45"/>
@@ -18684,7 +18702,7 @@
       <c r="J249" s="45"/>
       <c r="K249" s="54"/>
     </row>
-    <row r="250" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:11">
       <c r="B250" s="45"/>
       <c r="C250" s="45"/>
       <c r="D250" s="45"/>
@@ -18696,7 +18714,7 @@
       <c r="J250" s="45"/>
       <c r="K250" s="54"/>
     </row>
-    <row r="251" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="251" spans="2:11">
       <c r="B251" s="45"/>
       <c r="C251" s="45"/>
       <c r="D251" s="45"/>
@@ -18708,7 +18726,7 @@
       <c r="J251" s="45"/>
       <c r="K251" s="54"/>
     </row>
-    <row r="252" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:11">
       <c r="B252" s="45"/>
       <c r="C252" s="45"/>
       <c r="D252" s="45"/>
@@ -18720,7 +18738,7 @@
       <c r="J252" s="45"/>
       <c r="K252" s="54"/>
     </row>
-    <row r="253" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="253" spans="2:11">
       <c r="B253" s="45"/>
       <c r="C253" s="45"/>
       <c r="D253" s="45"/>
@@ -18732,7 +18750,7 @@
       <c r="J253" s="45"/>
       <c r="K253" s="54"/>
     </row>
-    <row r="254" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="254" spans="2:11">
       <c r="B254" s="45"/>
       <c r="C254" s="45"/>
       <c r="D254" s="45"/>
@@ -18744,7 +18762,7 @@
       <c r="J254" s="45"/>
       <c r="K254" s="54"/>
     </row>
-    <row r="255" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="255" spans="2:11">
       <c r="B255" s="45"/>
       <c r="C255" s="45"/>
       <c r="D255" s="45"/>
@@ -18756,7 +18774,7 @@
       <c r="J255" s="45"/>
       <c r="K255" s="54"/>
     </row>
-    <row r="256" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="256" spans="2:11">
       <c r="B256" s="45"/>
       <c r="C256" s="45"/>
       <c r="D256" s="45"/>
@@ -18768,7 +18786,7 @@
       <c r="J256" s="45"/>
       <c r="K256" s="54"/>
     </row>
-    <row r="257" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="257" spans="2:11">
       <c r="B257" s="45"/>
       <c r="C257" s="45"/>
       <c r="D257" s="45"/>
@@ -18780,7 +18798,7 @@
       <c r="J257" s="45"/>
       <c r="K257" s="54"/>
     </row>
-    <row r="258" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="258" spans="2:11">
       <c r="B258" s="45"/>
       <c r="C258" s="45"/>
       <c r="D258" s="45"/>
@@ -18792,7 +18810,7 @@
       <c r="J258" s="45"/>
       <c r="K258" s="54"/>
     </row>
-    <row r="259" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="259" spans="2:11">
       <c r="B259" s="45"/>
       <c r="C259" s="45"/>
       <c r="D259" s="45"/>
@@ -18804,7 +18822,7 @@
       <c r="J259" s="45"/>
       <c r="K259" s="54"/>
     </row>
-    <row r="260" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="260" spans="2:11">
       <c r="B260" s="45"/>
       <c r="C260" s="45"/>
       <c r="D260" s="45"/>
@@ -18816,7 +18834,7 @@
       <c r="J260" s="45"/>
       <c r="K260" s="54"/>
     </row>
-    <row r="261" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="261" spans="2:11">
       <c r="B261" s="45"/>
       <c r="C261" s="45"/>
       <c r="D261" s="45"/>
@@ -18828,7 +18846,7 @@
       <c r="J261" s="45"/>
       <c r="K261" s="54"/>
     </row>
-    <row r="262" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="262" spans="2:11">
       <c r="B262" s="45"/>
       <c r="C262" s="45"/>
       <c r="D262" s="45"/>
@@ -18840,7 +18858,7 @@
       <c r="J262" s="45"/>
       <c r="K262" s="54"/>
     </row>
-    <row r="263" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="263" spans="2:11">
       <c r="B263" s="45"/>
       <c r="C263" s="45"/>
       <c r="D263" s="45"/>
@@ -18852,7 +18870,7 @@
       <c r="J263" s="45"/>
       <c r="K263" s="54"/>
     </row>
-    <row r="264" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="264" spans="2:11">
       <c r="B264" s="45"/>
       <c r="C264" s="45"/>
       <c r="D264" s="45"/>
@@ -18864,7 +18882,7 @@
       <c r="J264" s="45"/>
       <c r="K264" s="54"/>
     </row>
-    <row r="265" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="265" spans="2:11">
       <c r="B265" s="45"/>
       <c r="C265" s="45"/>
       <c r="D265" s="45"/>
@@ -18876,7 +18894,7 @@
       <c r="J265" s="45"/>
       <c r="K265" s="54"/>
     </row>
-    <row r="266" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="266" spans="2:11">
       <c r="B266" s="45"/>
       <c r="C266" s="45"/>
       <c r="D266" s="45"/>
@@ -18888,7 +18906,7 @@
       <c r="J266" s="45"/>
       <c r="K266" s="54"/>
     </row>
-    <row r="267" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="267" spans="2:11">
       <c r="B267" s="45"/>
       <c r="C267" s="45"/>
       <c r="D267" s="45"/>
@@ -18900,7 +18918,7 @@
       <c r="J267" s="45"/>
       <c r="K267" s="54"/>
     </row>
-    <row r="268" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="268" spans="2:11">
       <c r="B268" s="45"/>
       <c r="C268" s="45"/>
       <c r="D268" s="45"/>
@@ -18912,7 +18930,7 @@
       <c r="J268" s="45"/>
       <c r="K268" s="54"/>
     </row>
-    <row r="269" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="269" spans="2:11">
       <c r="B269" s="45"/>
       <c r="C269" s="45"/>
       <c r="D269" s="45"/>
@@ -18925,7 +18943,6 @@
       <c r="K269" s="54"/>
     </row>
   </sheetData>
-  <autoFilter ref="C4:K208"/>
   <sortState ref="B5:K210">
     <sortCondition ref="C5:C210"/>
     <sortCondition ref="E5:E210"/>

</xml_diff>